<commit_message>
Backup QR Scanner data - 2025-12-28T08:53:47.879Z - Cache Bust: 1766912027879
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766911573720_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766911573720_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1222,9 +1222,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>201987</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C42" t="str">
+        <v>28/12/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>10:53:14</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F42" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-28T08:53:53.696Z - Cache Bust ID: 1766912033696tdrrgyu9s
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766911573720_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766911573720_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1222,29 +1222,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>201987</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C42" t="str">
-        <v>28/12/2025</v>
-      </c>
-      <c r="D42" t="str">
-        <v>10:53:14</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F42" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-29T08:54:35.824Z - Cache Bust: 1766998475824
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766911573720_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766911573720_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1222,9 +1222,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>201987</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C42" t="str">
+        <v>28/12/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>10:53:14</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F42" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>